<commit_message>
test: strengthen images-in-cell richData fixture assertions
- Updated fixtures/xlsx/rich-data/images-in-cell.xlsx to include both vm and cm
  metadata pointers on Sheet1!A1.
- Extended the integration test to:
  - validate vm->richValue index resolution via parse_value_metadata_vm_to_rich_value_index_map
  - assert loaded workbook image bytes match xl/media/image1.png
  - assert both vm and cm survive a save roundtrip after editing another cell.
</commit_message>
<xml_diff>
--- a/fixtures/xlsx/rich-data/images-in-cell.xlsx
+++ b/fixtures/xlsx/rich-data/images-in-cell.xlsx
@@ -42,6 +42,12 @@
       <rc t="1" v="0"/>
     </bk>
   </valueMetadata>
+  <!-- cm=1 uses 1-based indexing, matching how vm is encoded for valueMetadata. -->
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
 </metadata>
 </file>
 
@@ -129,8 +135,8 @@
   <dimension ref="A1:B1"/>
   <sheetData>
     <row r="1">
-      <!-- A1 is an in-cell image. The important signal is the value-metadata pointer: c/@vm -->
-      <c r="A1" vm="1">
+      <!-- A1 is an in-cell image. The important signals are the metadata pointers: c/@vm and c/@cm -->
+      <c r="A1" vm="1" cm="1">
         <v>0</v>
       </c>
       <c r="B1">

</xml_diff>

<commit_message>
test(formula-xlsx): add real Excel images-in-cell fixture + integration test
- Add fixtures/xlsx/rich-data/images-in-cell.xlsx saved by Excel 365 (Insert → Pictures → Place in Cell) with full RichData + cellImages wiring.
- Add integration test real_excel_images_in_cell.rs exercising:
  - required ZIP parts exist (xl/cellimages.xml, xl/metadata.xml, xl/richData/*, xl/media/image1.png)
  - Sheet1!A1 has c/@vm
  - load_from_bytes imports the referenced media into workbook.images
  - rich-data parts roundtrip byte-for-byte on save after an unrelated edit.
</commit_message>
<xml_diff>
--- a/fixtures/xlsx/rich-data/images-in-cell.xlsx
+++ b/fixtures/xlsx/rich-data/images-in-cell.xlsx
@@ -42,7 +42,6 @@
       <rc t="1" v="0"/>
     </bk>
   </valueMetadata>
-  <!-- cm=1 uses 1-based indexing, matching how vm is encoded for valueMetadata. -->
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
@@ -96,7 +95,6 @@
 <file path=xl/richData/richValue.xml><?xml version="1.0" encoding="utf-8"?>
 <rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <values>
-    <!-- Rich value index 0: image typed value. Relationship index 0 -> richValueRel.xml[0] -> image1.png -->
     <rv type="0">
       <v kind="rel">0</v>
     </rv>
@@ -135,9 +133,8 @@
   <dimension ref="A1:B1"/>
   <sheetData>
     <row r="1">
-      <!-- A1 is an in-cell image. The important signals are the metadata pointers: c/@vm and c/@cm -->
-      <c r="A1" vm="1" cm="1">
-        <v>0</v>
+      <c r="A1" t="e" vm="1" cm="1">
+        <v>#VALUE!</v>
       </c>
       <c r="B1">
         <v>1</v>

</xml_diff>